<commit_message>
First prototype of method converting sms submission to xml.
</commit_message>
<xml_diff>
--- a/test/sms_submission_converter/resources/sms_test_form.xlsx
+++ b/test/sms_submission_converter/resources/sms_test_form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -105,9 +105,15 @@
     <t xml:space="preserve">phonenumber</t>
   </si>
   <si>
+    <t xml:space="preserve">begin group</t>
+  </si>
+  <si>
     <t xml:space="preserve">note</t>
   </si>
   <si>
+    <t xml:space="preserve">nt</t>
+  </si>
+  <si>
     <t xml:space="preserve">note_title</t>
   </si>
   <si>
@@ -136,6 +142,9 @@
   </si>
   <si>
     <t xml:space="preserve">How many?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end group</t>
   </si>
   <si>
     <t xml:space="preserve">list name</t>
@@ -218,6 +227,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -226,14 +243,6 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -305,7 +314,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,7 +331,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,11 +343,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -416,12 +433,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ168"/>
+  <dimension ref="A1:AMJ169"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -431,12 +448,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="43.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="43.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="10.39"/>
   </cols>
   <sheetData>
@@ -607,16 +624,16 @@
       <c r="L8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -626,18 +643,16 @@
       <c r="K9" s="2"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -646,69 +661,96 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
-      <c r="AF10" s="2"/>
-      <c r="AG10" s="2"/>
-      <c r="AH10" s="2"/>
-      <c r="AI10" s="2"/>
-      <c r="AJ10" s="2"/>
-      <c r="AK10" s="2"/>
-      <c r="AL10" s="2"/>
-      <c r="AM10" s="2"/>
-      <c r="AN10" s="2"/>
-      <c r="AO10" s="2"/>
-      <c r="AP10" s="2"/>
-      <c r="AQ10" s="2"/>
-      <c r="AR10" s="2"/>
-      <c r="AS10" s="2"/>
-      <c r="AT10" s="2"/>
-      <c r="AU10" s="2"/>
-      <c r="AV10" s="2"/>
-      <c r="AW10" s="2"/>
-      <c r="AX10" s="2"/>
-      <c r="AY10" s="2"/>
-      <c r="AZ10" s="2"/>
-      <c r="BA10" s="2"/>
-      <c r="BB10" s="2"/>
-      <c r="BC10" s="2"/>
-      <c r="AMJ10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="2"/>
+      <c r="BA11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="2"/>
+      <c r="AMJ11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="B12" s="0" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="164" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="C12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="165" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -741,7 +783,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -752,24 +794,24 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,52 +1087,52 @@
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
-      <c r="C58" s="5"/>
+      <c r="C58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
-      <c r="C59" s="5"/>
+      <c r="C59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
-      <c r="C60" s="5"/>
+      <c r="C60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
-      <c r="C61" s="5"/>
+      <c r="C61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="5"/>
+      <c r="C62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
-      <c r="C63" s="5"/>
+      <c r="C63" s="7"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
-      <c r="C64" s="5"/>
+      <c r="C64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
-      <c r="C65" s="5"/>
+      <c r="C65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
-      <c r="C66" s="5"/>
+      <c r="C66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
-      <c r="C67" s="5"/>
+      <c r="C67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2"/>
@@ -1465,7 +1507,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1477,36 +1519,36 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>47</v>
       </c>
+      <c r="C1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="B2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>